<commit_message>
add register test case
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\eclipse-workspace\Batch24_Framework\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4902B8F-CFC6-4397-A957-0BBC2BB87F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,18 +19,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Test123@gmail.com</t>
   </si>
   <si>
     <t>123456sdx</t>
   </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>first@gmail</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -139,7 +139,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -174,7 +174,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -351,24 +351,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.08984375" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -379,12 +379,21 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{251A2776-DE7F-4A3F-A122-1717D57ADD13}"/>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>